<commit_message>
structure changes ready, updated bom
</commit_message>
<xml_diff>
--- a/domain/orders_example.xlsx
+++ b/domain/orders_example.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glebo\PycharmProjects\MagicDoors\domain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E03BEC-2FFE-4162-BA50-3B80C5825A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BDC7C8-9339-4EF5-979C-9C8D45B94892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" tabRatio="431" xr2:uid="{F19B50B0-3398-41C2-AE88-7F414EE9D6C2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" tabRatio="230" xr2:uid="{F19B50B0-3398-41C2-AE88-7F414EE9D6C2}"/>
   </bookViews>
   <sheets>
     <sheet name="1002" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -234,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -242,12 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -589,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5030672A-AC22-4F33-BAB3-2955DDF9779F}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B38" activeCellId="6" sqref="B3 B8 B13 B18 B25 B32 B38"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -632,19 +626,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -689,10 +683,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -700,15 +694,15 @@
       <c r="A7">
         <v>2</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
@@ -753,10 +747,10 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -764,15 +758,15 @@
       <c r="A12">
         <v>3</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
@@ -817,10 +811,10 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>17</v>
       </c>
     </row>
@@ -833,22 +827,22 @@
       <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18">
         <v>140</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18">
         <v>206</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18">
         <v>14</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" t="s">
         <v>8</v>
       </c>
       <c r="J18" t="s">
@@ -856,82 +850,55 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="3" t="s">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>5</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" t="s">
         <v>11</v>
       </c>
       <c r="D25">
@@ -943,10 +910,10 @@
       <c r="F25">
         <v>12</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" t="s">
         <v>8</v>
       </c>
       <c r="J25" t="s">
@@ -954,42 +921,42 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B26" s="3" t="s">
+      <c r="B26" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B27" s="3" t="s">
+      <c r="B27" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B28" s="3" t="s">
+      <c r="B28" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B29" s="3" t="s">
+      <c r="B29" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B30" s="3" t="s">
+      <c r="B30" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" t="s">
         <v>17</v>
       </c>
     </row>
@@ -997,14 +964,12 @@
       <c r="A31">
         <v>6</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" t="s">
         <v>11</v>
       </c>
       <c r="D32">
@@ -1016,13 +981,13 @@
       <c r="F32">
         <v>10</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H32" t="s">
         <v>8</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="4">
         <v>1.7</v>
       </c>
       <c r="J32" t="s">
@@ -1030,34 +995,34 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B33" s="3" t="s">
+      <c r="B33" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B34" s="3" t="s">
+      <c r="B34" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B35" s="3" t="s">
+      <c r="B35" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B36" s="3" t="s">
+      <c r="B36" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1065,14 +1030,12 @@
       <c r="A37">
         <v>7</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" t="s">
         <v>11</v>
       </c>
       <c r="D38">
@@ -1084,13 +1047,13 @@
       <c r="F38">
         <v>10</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="G38" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" t="s">
         <v>8</v>
       </c>
-      <c r="I38" s="7">
+      <c r="I38" s="4">
         <v>1.7</v>
       </c>
       <c r="J38" t="s">
@@ -1098,50 +1061,50 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B39" s="3" t="s">
+      <c r="B39" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B40" s="3" t="s">
+      <c r="B40" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B41" s="3" t="s">
+      <c r="B41" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B42" s="3" t="s">
+      <c r="B42" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B43" s="3" t="s">
+      <c r="B43" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B44" s="3" t="s">
+      <c r="B44" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1149,14 +1112,12 @@
       <c r="A45">
         <v>8</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B46" s="3" t="s">
+      <c r="B46" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" t="s">
         <v>43</v>
       </c>
       <c r="D46">
@@ -1168,10 +1129,10 @@
       <c r="F46">
         <v>12</v>
       </c>
-      <c r="G46" s="6" t="s">
+      <c r="G46" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H46" t="s">
         <v>8</v>
       </c>
       <c r="J46" t="s">
@@ -1179,10 +1140,10 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B47" s="3" t="s">
+      <c r="B47" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>